<commit_message>
add JSON line parsing option
</commit_message>
<xml_diff>
--- a/tests/test_files/file.xlsx
+++ b/tests/test_files/file.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Wikit\Chunk_Norris\chunknorris\tests\test_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Wikit\Improvement_Retrieval\ChunkNorris\chunknorris\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57D7EAD4-2B6E-4448-B627-AD85F550CA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F123636B-2AF2-48E8-AF1A-78C3CA47BAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="19200" windowHeight="11170" activeTab="1" xr2:uid="{3F93D3C5-5DCD-488E-8F41-FCC97486122E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{3F93D3C5-5DCD-488E-8F41-FCC97486122E}"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="CSV-like" sheetId="1" r:id="rId1"/>
+    <sheet name="Not CSV-like" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Training id</t>
   </si>
@@ -81,6 +81,33 @@
   </si>
   <si>
     <t>High variance, tuning required.</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>Bonjour</t>
+  </si>
+  <si>
+    <t>Buongiorno</t>
+  </si>
+  <si>
+    <t>Hey</t>
+  </si>
+  <si>
+    <t>Salut</t>
+  </si>
+  <si>
+    <t>Bad bad bad</t>
+  </si>
+  <si>
+    <t>Good Good Good</t>
   </si>
 </sst>
 </file>
@@ -404,7 +431,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -682,6 +709,43 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -738,7 +802,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -767,14 +831,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1207,16 +1280,16 @@
       <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="7">
         <v>100</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1227,14 +1300,14 @@
       <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="12">
+      <c r="D4" s="13"/>
+      <c r="E4" s="7">
         <v>400</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1245,30 +1318,30 @@
       <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="14">
+      <c r="D6" s="14"/>
+      <c r="E6" s="8">
         <v>50</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1288,7 +1361,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1301,56 +1374,48 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="B1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="9">
-        <v>1</v>
+      <c r="A2" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="10">
-        <v>200</v>
+        <v>24</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="7">
         <v>100</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1358,51 +1423,47 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="11">
-        <v>3</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="12">
-        <v>400</v>
+      <c r="C4" s="7"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="7">
+        <v>100</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="12"/>
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="14">
+      <c r="D6" s="14"/>
+      <c r="E6" s="8">
         <v>50</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1410,8 +1471,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D3:D6"/>
+    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add JSON line parsing option (#45)
Co-authored-by: Mathieu Ciancone <mathieu@wikit.ai>
</commit_message>
<xml_diff>
--- a/tests/test_files/file.xlsx
+++ b/tests/test_files/file.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Wikit\Chunk_Norris\chunknorris\tests\test_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Wikit\Improvement_Retrieval\ChunkNorris\chunknorris\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57D7EAD4-2B6E-4448-B627-AD85F550CA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F123636B-2AF2-48E8-AF1A-78C3CA47BAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="19200" windowHeight="11170" activeTab="1" xr2:uid="{3F93D3C5-5DCD-488E-8F41-FCC97486122E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{3F93D3C5-5DCD-488E-8F41-FCC97486122E}"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="CSV-like" sheetId="1" r:id="rId1"/>
+    <sheet name="Not CSV-like" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Training id</t>
   </si>
@@ -81,6 +81,33 @@
   </si>
   <si>
     <t>High variance, tuning required.</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>Bonjour</t>
+  </si>
+  <si>
+    <t>Buongiorno</t>
+  </si>
+  <si>
+    <t>Hey</t>
+  </si>
+  <si>
+    <t>Salut</t>
+  </si>
+  <si>
+    <t>Bad bad bad</t>
+  </si>
+  <si>
+    <t>Good Good Good</t>
   </si>
 </sst>
 </file>
@@ -404,7 +431,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -682,6 +709,43 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -738,7 +802,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -767,14 +831,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1207,16 +1280,16 @@
       <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="7">
         <v>100</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1227,14 +1300,14 @@
       <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="12">
+      <c r="D4" s="13"/>
+      <c r="E4" s="7">
         <v>400</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1245,30 +1318,30 @@
       <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="14">
+      <c r="D6" s="14"/>
+      <c r="E6" s="8">
         <v>50</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1288,7 +1361,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1301,56 +1374,48 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="B1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="9">
-        <v>1</v>
+      <c r="A2" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="10">
-        <v>200</v>
+        <v>24</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="7">
         <v>100</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1358,51 +1423,47 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="11">
-        <v>3</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="12">
-        <v>400</v>
+      <c r="C4" s="7"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="7">
+        <v>100</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="12"/>
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="14">
+      <c r="D6" s="14"/>
+      <c r="E6" s="8">
         <v>50</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1410,8 +1471,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D3:D6"/>
+    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>